<commit_message>
Added tds feature and edit view of invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v5.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v5.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>{meta:invoice_type}</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>{meta:sub_service_cost}</t>
+  </si>
+  <si>
+    <t>Tax Deducted @ {meta:tds_tax_rate}</t>
+  </si>
+  <si>
+    <t>{meta:tds}</t>
   </si>
   <si>
     <t>GRAND TOTAL</t>
@@ -377,16 +383,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -453,7 +456,7 @@
     <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -493,9 +496,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -527,54 +527,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
@@ -582,206 +582,206 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6">
       <c r="A6" s="1"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="1"/>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8">
       <c r="A8" s="1"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="1"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12">
       <c r="A12" s="1"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14">
       <c r="A14" s="1"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="23" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="1"/>
@@ -791,28 +791,28 @@
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="16">
         <v>0.0</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="25" t="s">
         <v>27</v>
       </c>
       <c r="J16" s="1"/>
@@ -822,14 +822,14 @@
     </row>
     <row r="17">
       <c r="A17" s="1"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="15"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -837,14 +837,14 @@
     </row>
     <row r="18">
       <c r="A18" s="1"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="29"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -852,18 +852,18 @@
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="33" t="s">
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="32" t="s">
         <v>30</v>
       </c>
       <c r="J19" s="1"/>
@@ -873,20 +873,20 @@
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -894,14 +894,14 @@
     </row>
     <row r="21">
       <c r="A21" s="1"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="15"/>
+      <c r="I21" s="14"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -909,10 +909,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="16">
         <v>14.0</v>
       </c>
       <c r="D22" s="1"/>
@@ -920,7 +920,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="26" t="s">
+      <c r="I22" s="25" t="s">
         <v>35</v>
       </c>
       <c r="J22" s="1"/>
@@ -930,10 +930,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1"/>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="16">
         <v>0.5</v>
       </c>
       <c r="D23" s="1"/>
@@ -941,7 +941,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="25" t="s">
         <v>37</v>
       </c>
       <c r="J23" s="1"/>
@@ -951,10 +951,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1"/>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="16">
         <v>0.5</v>
       </c>
       <c r="D24" s="1"/>
@@ -962,7 +962,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="26" t="s">
+      <c r="I24" s="25" t="s">
         <v>37</v>
       </c>
       <c r="J24" s="1"/>
@@ -972,14 +972,14 @@
     </row>
     <row r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="15"/>
+      <c r="I25" s="14"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -987,18 +987,18 @@
     </row>
     <row r="26">
       <c r="A26" s="1"/>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37" t="s">
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="38" t="s">
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="37" t="s">
         <v>41</v>
       </c>
       <c r="J26" s="1"/>
@@ -1008,16 +1008,16 @@
     </row>
     <row r="27">
       <c r="A27" s="1"/>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
       <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="24" t="s">
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="37" t="s">
         <v>43</v>
       </c>
       <c r="J27" s="1"/>
@@ -1027,14 +1027,18 @@
     </row>
     <row r="28">
       <c r="A28" s="1"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="15"/>
+      <c r="B28" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1042,13 +1046,14 @@
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="B29" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="15"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="14"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1056,14 +1061,13 @@
     </row>
     <row r="30">
       <c r="A30" s="1"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="42"/>
+      <c r="B30" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" s="14"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1071,20 +1075,35 @@
     </row>
     <row r="31">
       <c r="A31" s="1"/>
-      <c r="B31" s="43" t="s">
-        <v>46</v>
-      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="40"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
+    <row r="32">
+      <c r="A32" s="1"/>
+      <c r="B32" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:H30"/>
-    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="B32:I32"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove TDS from main invoice template
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v5.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v5.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>{meta:invoice_type}</t>
   </si>
@@ -137,12 +137,6 @@
   </si>
   <si>
     <t>{meta:sub_service_cost}</t>
-  </si>
-  <si>
-    <t>Tax Deducted @ {meta:tds_tax_rate}</t>
-  </si>
-  <si>
-    <t>{meta:tds}</t>
   </si>
   <si>
     <t>GRAND TOTAL</t>
@@ -1008,16 +1002,16 @@
     </row>
     <row r="27">
       <c r="A27" s="1"/>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="37" t="s">
+      <c r="I27" s="23" t="s">
         <v>43</v>
       </c>
       <c r="J27" s="1"/>
@@ -1027,18 +1021,14 @@
     </row>
     <row r="28">
       <c r="A28" s="1"/>
-      <c r="B28" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="14"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1046,13 +1036,12 @@
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="B29" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>45</v>
+      </c>
       <c r="I29" s="14"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1061,13 +1050,14 @@
     </row>
     <row r="30">
       <c r="A30" s="1"/>
-      <c r="B30" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="14"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="40"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1075,35 +1065,20 @@
     </row>
     <row r="31">
       <c r="A31" s="1"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
+      <c r="B31" s="41" t="s">
+        <v>46</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32">
-      <c r="A32" s="1"/>
-      <c r="B32" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:H31"/>
-    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:H30"/>
+    <mergeCell ref="B31:I31"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Round used in Invoices for ST and VAT
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v5.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-FoC-v5.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>{meta:invoice_type}</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>VAT</t>
-  </si>
-  <si>
-    <t>{meta:vat_tax}</t>
   </si>
   <si>
     <t>{meta:part_cost_vat}</t>
@@ -536,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -703,6 +700,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -984,7 +984,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1241,7 +1241,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="37" t="s">
         <v>14</v>
@@ -1250,16 +1250,16 @@
         <v>15</v>
       </c>
       <c r="F15" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="I15" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="H15" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1325,13 +1325,13 @@
       <c r="B18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>29</v>
+      <c r="C18" s="57">
+        <v>5</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="39"/>
       <c r="F18" s="40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
@@ -1359,7 +1359,7 @@
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="40">
         <v>14</v>
@@ -1370,7 +1370,7 @@
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1380,7 +1380,7 @@
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="40">
         <v>0.5</v>
@@ -1391,7 +1391,7 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1401,7 +1401,7 @@
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="40">
         <v>0.5</v>
@@ -1412,7 +1412,7 @@
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1437,20 +1437,20 @@
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="40" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1460,7 +1460,7 @@
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
@@ -1469,7 +1469,7 @@
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1494,10 +1494,10 @@
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
@@ -1528,7 +1528,7 @@
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="52"/>
       <c r="D29" s="52"/>

</xml_diff>